<commit_message>
Code Runs with New observables
</commit_message>
<xml_diff>
--- a/08_Pronóstico/Datos/DataCOL.xlsx
+++ b/08_Pronóstico/Datos/DataCOL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarincong/Documents/Git Repos/CAEP/08_Pronóstico/Datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A652A2D2-39B9-E34F-AC28-9DC5B4459EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE9A620-A3C8-7D47-83EB-96D5D7C5B400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28080" windowHeight="21100" xr2:uid="{3B812F19-A572-41B0-90ED-022F2B941229}"/>
   </bookViews>
@@ -37,6 +37,15 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+  <si>
+    <t>Y_obs</t>
+  </si>
+  <si>
+    <t>C_obs</t>
+  </si>
+  <si>
+    <t>I_obs</t>
+  </si>
   <si>
     <t>Y</t>
   </si>
@@ -78,15 +87,6 @@
   </si>
   <si>
     <t>pi</t>
-  </si>
-  <si>
-    <t>Y_hat</t>
-  </si>
-  <si>
-    <t>C_hat</t>
-  </si>
-  <si>
-    <t>I_hat</t>
   </si>
   <si>
     <t>log_Y_hat</t>
@@ -476,9 +476,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC43C700-5E37-433E-91EB-5805D755A630}">
   <dimension ref="A1:AC111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="150" zoomScaleNormal="160" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -503,52 +503,52 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>0</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>1</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>2</v>
-      </c>
-      <c r="N1" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" t="s">
-        <v>16</v>
       </c>
       <c r="Q1" t="s">
         <v>17</v>
@@ -560,7 +560,7 @@
         <v>19</v>
       </c>
       <c r="T1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="X1" s="3"/>
       <c r="Y1" s="3"/>

</xml_diff>

<commit_message>
Adds observable for foreign demand
1. Variable definition: y_star_obs
2. Measurement equation: y_star_obs = y_star
3. Observable
</commit_message>
<xml_diff>
--- a/08_Pronóstico/Datos/DataCOL.xlsx
+++ b/08_Pronóstico/Datos/DataCOL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarincong/Documents/Git Repos/CAEP/08_Pronóstico/Datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE9A620-A3C8-7D47-83EB-96D5D7C5B400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C223D4D2-2AE7-CB4D-B5C2-3C216229AFD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28080" windowHeight="21100" xr2:uid="{3B812F19-A572-41B0-90ED-022F2B941229}"/>
+    <workbookView xWindow="0" yWindow="1000" windowWidth="28080" windowHeight="21100" xr2:uid="{3B812F19-A572-41B0-90ED-022F2B941229}"/>
   </bookViews>
   <sheets>
     <sheet name="Data_Col" sheetId="1" r:id="rId1"/>
@@ -74,9 +74,6 @@
     <t>Dates</t>
   </si>
   <si>
-    <t>y_star_hat</t>
-  </si>
-  <si>
     <t>log_y_star_hat</t>
   </si>
   <si>
@@ -96,6 +93,9 @@
   </si>
   <si>
     <t>log_I_hat</t>
+  </si>
+  <si>
+    <t>y_star_obs</t>
   </si>
 </sst>
 </file>
@@ -476,9 +476,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC43C700-5E37-433E-91EB-5805D755A630}">
   <dimension ref="A1:AC111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="150" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N17" sqref="N17"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -509,28 +509,28 @@
         <v>8</v>
       </c>
       <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
         <v>12</v>
-      </c>
-      <c r="D1" t="s">
-        <v>13</v>
       </c>
       <c r="E1" t="s">
         <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G1" t="s">
         <v>7</v>
       </c>
       <c r="H1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I1" t="s">
         <v>9</v>
       </c>
       <c r="J1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K1" t="s">
         <v>3</v>
@@ -551,13 +551,13 @@
         <v>2</v>
       </c>
       <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
         <v>17</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>18</v>
-      </c>
-      <c r="S1" t="s">
-        <v>19</v>
       </c>
       <c r="T1" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Added Foreign Inflation and Observable discrepancies
</commit_message>
<xml_diff>
--- a/08_Pronóstico/Datos/DataCOL.xlsx
+++ b/08_Pronóstico/Datos/DataCOL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarincong/Documents/Git Repos/CAEP/08_Pronóstico/Datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C223D4D2-2AE7-CB4D-B5C2-3C216229AFD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25809335-62DA-1942-8FC1-37161864BF17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1000" windowWidth="28080" windowHeight="21100" xr2:uid="{3B812F19-A572-41B0-90ED-022F2B941229}"/>
   </bookViews>
@@ -77,9 +77,6 @@
     <t>log_y_star_hat</t>
   </si>
   <si>
-    <t>pi_star</t>
-  </si>
-  <si>
     <t>pi_im_star</t>
   </si>
   <si>
@@ -96,6 +93,9 @@
   </si>
   <si>
     <t>y_star_obs</t>
+  </si>
+  <si>
+    <t>pi_star_obs</t>
   </si>
 </sst>
 </file>
@@ -478,7 +478,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -509,7 +509,7 @@
         <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
         <v>12</v>
@@ -518,19 +518,19 @@
         <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="G1" t="s">
         <v>7</v>
       </c>
       <c r="H1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I1" t="s">
         <v>9</v>
       </c>
       <c r="J1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K1" t="s">
         <v>3</v>
@@ -551,13 +551,13 @@
         <v>2</v>
       </c>
       <c r="Q1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
       </c>
       <c r="T1" t="s">
         <v>10</v>
@@ -639,7 +639,7 @@
         <v>172.2</v>
       </c>
       <c r="F3" s="8">
-        <f>E3/E2-1</f>
+        <f>(E3/E2-1)</f>
         <v>7.0175438596491446E-3</v>
       </c>
       <c r="G3" s="8">
@@ -7181,6 +7181,7 @@
     </row>
     <row r="105" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A105" s="1"/>
+      <c r="F105" s="8"/>
     </row>
     <row r="106" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A106" s="1"/>

</xml_diff>

<commit_message>
Added imports price inflation in foreign currency
+ Measurement error
+ SS bias
</commit_message>
<xml_diff>
--- a/08_Pronóstico/Datos/DataCOL.xlsx
+++ b/08_Pronóstico/Datos/DataCOL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarincong/Documents/Git Repos/CAEP/08_Pronóstico/Datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25809335-62DA-1942-8FC1-37161864BF17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C8A2E3-B591-5948-BCB2-F962FC15B98B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1000" windowWidth="28080" windowHeight="21100" xr2:uid="{3B812F19-A572-41B0-90ED-022F2B941229}"/>
   </bookViews>
@@ -77,9 +77,6 @@
     <t>log_y_star_hat</t>
   </si>
   <si>
-    <t>pi_im_star</t>
-  </si>
-  <si>
     <t>pi</t>
   </si>
   <si>
@@ -96,6 +93,9 @@
   </si>
   <si>
     <t>pi_star_obs</t>
+  </si>
+  <si>
+    <t>pi_im_star_obs</t>
   </si>
 </sst>
 </file>
@@ -478,7 +478,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -489,7 +489,7 @@
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" customWidth="1"/>
+    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
     <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
@@ -509,7 +509,7 @@
         <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
         <v>12</v>
@@ -518,19 +518,19 @@
         <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G1" t="s">
         <v>7</v>
       </c>
       <c r="H1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="I1" t="s">
         <v>9</v>
       </c>
       <c r="J1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K1" t="s">
         <v>3</v>
@@ -551,13 +551,13 @@
         <v>2</v>
       </c>
       <c r="Q1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>16</v>
-      </c>
-      <c r="S1" t="s">
-        <v>17</v>
       </c>
       <c r="T1" t="s">
         <v>10</v>
@@ -7203,5 +7203,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed Filtered Observables for Log transformations
</commit_message>
<xml_diff>
--- a/08_Pronóstico/Datos/DataCOL.xlsx
+++ b/08_Pronóstico/Datos/DataCOL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarincong/Documents/Git Repos/CAEP/08_Pronóstico/Datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C8A2E3-B591-5948-BCB2-F962FC15B98B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{991E9AE8-93F8-9943-87C5-508AEDEF052B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1000" windowWidth="28080" windowHeight="21100" xr2:uid="{3B812F19-A572-41B0-90ED-022F2B941229}"/>
   </bookViews>
@@ -74,19 +74,7 @@
     <t>Dates</t>
   </si>
   <si>
-    <t>log_y_star_hat</t>
-  </si>
-  <si>
     <t>pi</t>
-  </si>
-  <si>
-    <t>log_Y_hat</t>
-  </si>
-  <si>
-    <t>log_C_hat</t>
-  </si>
-  <si>
-    <t>log_I_hat</t>
   </si>
   <si>
     <t>y_star_obs</t>
@@ -96,6 +84,18 @@
   </si>
   <si>
     <t>pi_im_star_obs</t>
+  </si>
+  <si>
+    <t>y_star_obs Lev</t>
+  </si>
+  <si>
+    <t>Y_obs Lev</t>
+  </si>
+  <si>
+    <t>C_obs Lev</t>
+  </si>
+  <si>
+    <t>I_obs Lev</t>
   </si>
 </sst>
 </file>
@@ -476,9 +476,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC43C700-5E37-433E-91EB-5805D755A630}">
   <dimension ref="A1:AC111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="150" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
+      <selection pane="bottomLeft" activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -509,28 +509,28 @@
         <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E1" t="s">
         <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G1" t="s">
         <v>7</v>
       </c>
       <c r="H1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I1" t="s">
         <v>9</v>
       </c>
       <c r="J1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K1" t="s">
         <v>3</v>
@@ -542,22 +542,22 @@
         <v>5</v>
       </c>
       <c r="N1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
         <v>0</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>1</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>2</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" t="s">
-        <v>16</v>
       </c>
       <c r="T1" t="s">
         <v>10</v>
@@ -616,7 +616,7 @@
         <v>1.6795963668217E-2</v>
       </c>
       <c r="S2" s="8">
-        <v>1021.5965546112</v>
+        <v>4.4572212024318998E-2</v>
       </c>
       <c r="T2" s="8">
         <v>0.12</v>
@@ -681,7 +681,7 @@
         <v>1.2671168300593999E-2</v>
       </c>
       <c r="S3" s="8">
-        <v>595.49760919097901</v>
+        <v>1.9406443418518E-2</v>
       </c>
       <c r="T3" s="8">
         <v>0.12</v>
@@ -746,7 +746,7 @@
         <v>1.0391471298094E-2</v>
       </c>
       <c r="S4" s="8">
-        <v>253.16855482395599</v>
+        <v>1.9471916319700001E-4</v>
       </c>
       <c r="T4" s="8">
         <v>0.12</v>
@@ -818,7 +818,7 @@
         <v>1.0148409321724E-2</v>
       </c>
       <c r="S5" s="8">
-        <v>-667.36189694775499</v>
+        <v>-6.0480361725084003E-2</v>
       </c>
       <c r="T5" s="8">
         <v>0.12</v>
@@ -883,7 +883,7 @@
         <v>8.7351076065529994E-3</v>
       </c>
       <c r="S6" s="8">
-        <v>-390.39454144872599</v>
+        <v>-3.5262961891975003E-2</v>
       </c>
       <c r="T6" s="8">
         <v>0.11888888888888889</v>
@@ -948,7 +948,7 @@
         <v>5.236172305498E-3</v>
       </c>
       <c r="S7" s="8">
-        <v>183.43954359564401</v>
+        <v>7.2302450906110002E-3</v>
       </c>
       <c r="T7" s="8">
         <v>0.115</v>
@@ -1013,7 +1013,7 @@
         <v>5.3022895271799997E-4</v>
       </c>
       <c r="S8" s="8">
-        <v>366.92022528693798</v>
+        <v>2.1472454326681999E-2</v>
       </c>
       <c r="T8" s="8">
         <v>0.10592391304347826</v>
@@ -1078,7 +1078,7 @@
         <v>3.1681587112370002E-3</v>
       </c>
       <c r="S9" s="8">
-        <v>-294.09122151895201</v>
+        <v>-1.7823613695734E-2</v>
       </c>
       <c r="T9" s="8">
         <v>8.983695652173912E-2</v>
@@ -1143,7 +1143,7 @@
         <v>-7.4303514995260004E-3</v>
       </c>
       <c r="S10" s="8">
-        <v>-1159.51509272765</v>
+        <v>-7.0301711863580002E-2</v>
       </c>
       <c r="T10" s="8">
         <v>7.9944444444444443E-2</v>
@@ -1208,7 +1208,7 @@
         <v>-7.7862408232540004E-3</v>
       </c>
       <c r="S11" s="8">
-        <v>988.94461086202102</v>
+        <v>6.1078376025932003E-2</v>
       </c>
       <c r="T11" s="8">
         <v>6.0961538461538456E-2</v>
@@ -1273,7 +1273,7 @@
         <v>-3.2951772995999997E-5</v>
       </c>
       <c r="S12" s="8">
-        <v>51.050190578233</v>
+        <v>8.4501843300440003E-3</v>
       </c>
       <c r="T12" s="8">
         <v>5.2499999999999998E-2</v>
@@ -1338,7 +1338,7 @@
         <v>-1.5244063964012001E-2</v>
       </c>
       <c r="S13" s="8">
-        <v>-246.91476376828001</v>
+        <v>-7.4730955018420002E-3</v>
       </c>
       <c r="T13" s="8">
         <v>5.2499999999999998E-2</v>
@@ -1403,7 +1403,7 @@
         <v>-1.9841436957737001E-2</v>
       </c>
       <c r="S14" s="8">
-        <v>78.7193064847378</v>
+        <v>1.1480360382841E-2</v>
       </c>
       <c r="T14" s="8">
         <v>6.0388888888888888E-2</v>
@@ -1468,7 +1468,7 @@
         <v>-1.3168332088218999E-2</v>
       </c>
       <c r="S15" s="8">
-        <v>104.74376371853501</v>
+        <v>1.3277730237283E-2</v>
       </c>
       <c r="T15" s="8">
         <v>6.9423076923076921E-2</v>
@@ -1533,7 +1533,7 @@
         <v>-8.6955682234000006E-3</v>
       </c>
       <c r="S16" s="8">
-        <v>-916.12919815600605</v>
+        <v>-4.0656091837704002E-2</v>
       </c>
       <c r="T16" s="8">
         <v>7.2499999999999995E-2</v>
@@ -1598,7 +1598,7 @@
         <v>-7.9409614888610001E-3</v>
       </c>
       <c r="S17" s="8">
-        <v>722.36265238072804</v>
+        <v>4.4259642755578997E-2</v>
       </c>
       <c r="T17" s="8">
         <v>7.2499999999999995E-2</v>
@@ -1663,7 +1663,7 @@
         <v>-3.7245266393009999E-3</v>
       </c>
       <c r="S18" s="8">
-        <v>382.06883178775303</v>
+        <v>2.7177904879203001E-2</v>
       </c>
       <c r="T18" s="8">
         <v>7.12087912087912E-2</v>
@@ -1728,7 +1728,7 @@
         <v>-1.1736570183126E-2</v>
       </c>
       <c r="S19" s="8">
-        <v>-721.39012219922301</v>
+        <v>-2.6811891024040999E-2</v>
       </c>
       <c r="T19" s="8">
         <v>6.7500000000000004E-2</v>
@@ -1793,7 +1793,7 @@
         <v>-1.4445730885550999E-2</v>
       </c>
       <c r="S20" s="8">
-        <v>-145.13419916822301</v>
+        <v>1.7174206288179999E-3</v>
       </c>
       <c r="T20" s="8">
         <v>6.7500000000000004E-2</v>
@@ -1858,7 +1858,7 @@
         <v>-6.2545342299800001E-4</v>
       </c>
       <c r="S21" s="8">
-        <v>924.60675742593196</v>
+        <v>5.0027410444799997E-2</v>
       </c>
       <c r="T21" s="8">
         <v>6.7173913043478264E-2</v>
@@ -1923,7 +1923,7 @@
         <v>-1.054406289399E-2</v>
       </c>
       <c r="S22" s="8">
-        <v>339.39081059963701</v>
+        <v>2.3459125387131002E-2</v>
       </c>
       <c r="T22" s="8">
         <v>6.5000000000000002E-2</v>
@@ -1988,7 +1988,7 @@
         <v>-1.654465732653E-3</v>
       </c>
       <c r="S23" s="8">
-        <v>-2243.2519009211101</v>
+        <v>-9.4896422308285003E-2</v>
       </c>
       <c r="T23" s="8">
         <v>6.5000000000000002E-2</v>
@@ -2053,7 +2053,7 @@
         <v>-1.1784835426464E-2</v>
       </c>
       <c r="S24" s="8">
-        <v>-2935.9608259547299</v>
+        <v>-0.125752215215929</v>
       </c>
       <c r="T24" s="8">
         <v>6.4347826086956522E-2</v>
@@ -2118,7 +2118,7 @@
         <v>-9.2547937834979999E-3</v>
       </c>
       <c r="S25" s="8">
-        <v>-1968.11934897948</v>
+        <v>-7.7857762172482997E-2</v>
       </c>
       <c r="T25" s="8">
         <v>0.06</v>
@@ -2183,7 +2183,7 @@
         <v>4.2283597460399997E-4</v>
       </c>
       <c r="S26" s="8">
-        <v>-370.92333362926001</v>
+        <v>-8.0814204638050002E-3</v>
       </c>
       <c r="T26" s="8">
         <v>0.06</v>
@@ -2248,7 +2248,7 @@
         <v>7.2295423400310001E-3</v>
       </c>
       <c r="S27" s="8">
-        <v>-929.52445351208701</v>
+        <v>-3.1050524805776001E-2</v>
       </c>
       <c r="T27" s="8">
         <v>6.1923076923076928E-2</v>
@@ -2313,7 +2313,7 @@
         <v>5.6823362056679996E-3</v>
       </c>
       <c r="S28" s="8">
-        <v>24.799081735262</v>
+        <v>6.8037648934599999E-3</v>
       </c>
       <c r="T28" s="8">
         <v>6.6086956521739126E-2</v>
@@ -2378,7 +2378,7 @@
         <v>5.3695122212079997E-3</v>
       </c>
       <c r="S29" s="8">
-        <v>1333.16148183118</v>
+        <v>5.4375537564084003E-2</v>
       </c>
       <c r="T29" s="8">
         <v>7.2065217391304351E-2</v>
@@ -2443,7 +2443,7 @@
         <v>1.0170272979238001E-2</v>
       </c>
       <c r="S30" s="8">
-        <v>3791.2800246174802</v>
+        <v>0.13582199472214801</v>
       </c>
       <c r="T30" s="8">
         <v>7.7833333333333338E-2</v>
@@ -2508,7 +2508,7 @@
         <v>1.2822778005788E-2</v>
       </c>
       <c r="S31" s="8">
-        <v>2835.43557333128</v>
+        <v>0.10145767999329899</v>
       </c>
       <c r="T31" s="8">
         <v>8.5576923076923078E-2</v>
@@ -2573,7 +2573,7 @@
         <v>2.2989143488825001E-2</v>
       </c>
       <c r="S32" s="8">
-        <v>2534.4855700466501</v>
+        <v>8.902746374612E-2</v>
       </c>
       <c r="T32" s="8">
         <v>9.1711956521739121E-2</v>
@@ -2638,7 +2638,7 @@
         <v>2.154369813695E-2</v>
       </c>
       <c r="S33" s="8">
-        <v>1966.3847546992999</v>
+        <v>6.8329293683734998E-2</v>
       </c>
       <c r="T33" s="8">
         <v>9.3478260869565219E-2</v>
@@ -2703,7 +2703,7 @@
         <v>1.5057092175224E-2</v>
       </c>
       <c r="S34" s="8">
-        <v>320.296329155688</v>
+        <v>1.222799228748E-2</v>
       </c>
       <c r="T34" s="8">
         <v>9.5989010989010984E-2</v>
@@ -2768,7 +2768,7 @@
         <v>1.1396618494880001E-2</v>
       </c>
       <c r="S35" s="8">
-        <v>217.49269247617801</v>
+        <v>8.1116376861839999E-3</v>
       </c>
       <c r="T35" s="8">
         <v>9.7500000000000003E-2</v>
@@ -2833,7 +2833,7 @@
         <v>9.8633147883439992E-3</v>
       </c>
       <c r="S36" s="8">
-        <v>-503.02184574056002</v>
+        <v>-1.6300060933537999E-2</v>
       </c>
       <c r="T36" s="8">
         <v>9.9266304347826087E-2</v>
@@ -2898,7 +2898,7 @@
         <v>8.0632280312929999E-3</v>
       </c>
       <c r="S37" s="8">
-        <v>-916.16922257580097</v>
+        <v>-2.9948846171877999E-2</v>
       </c>
       <c r="T37" s="8">
         <v>9.945652173913043E-2</v>
@@ -2963,7 +2963,7 @@
         <v>-4.7690003370580002E-3</v>
       </c>
       <c r="S38" s="8">
-        <v>-519.15926128375895</v>
+        <v>-1.6511180945442998E-2</v>
       </c>
       <c r="T38" s="8">
         <v>8.7555555555555567E-2</v>
@@ -3028,7 +3028,7 @@
         <v>-1.1008298851095E-2</v>
       </c>
       <c r="S39" s="8">
-        <v>-777.64292351953895</v>
+        <v>-2.4435138828756999E-2</v>
       </c>
       <c r="T39" s="8">
         <v>5.9890109890109892E-2</v>
@@ -3093,7 +3093,7 @@
         <v>-1.7239383386304E-2</v>
       </c>
       <c r="S40" s="8">
-        <v>-763.17461735710799</v>
+        <v>-2.3372154135849001E-2</v>
       </c>
       <c r="T40" s="8">
         <v>4.4836956521739128E-2</v>
@@ -3158,7 +3158,7 @@
         <v>-2.0767461818506E-2</v>
       </c>
       <c r="S41" s="8">
-        <v>-2209.8890936156499</v>
+        <v>-6.8606515390745998E-2</v>
       </c>
       <c r="T41" s="8">
         <v>3.7934782608695657E-2</v>
@@ -3223,7 +3223,7 @@
         <v>-1.2707008424433E-2</v>
       </c>
       <c r="S42" s="8">
-        <v>-1923.46556036383</v>
+        <v>-5.7945725313584003E-2</v>
       </c>
       <c r="T42" s="8">
         <v>3.5000000000000003E-2</v>
@@ -3288,7 +3288,7 @@
         <v>-1.3098267508555E-2</v>
       </c>
       <c r="S43" s="8">
-        <v>-970.50658369841403</v>
+        <v>-2.7417736635119001E-2</v>
       </c>
       <c r="T43" s="8">
         <v>3.1758241758241754E-2</v>
@@ -3353,7 +3353,7 @@
         <v>-9.8085946258810001E-3</v>
       </c>
       <c r="S44" s="8">
-        <v>-1723.41564060366</v>
+        <v>-4.9044344492505998E-2</v>
       </c>
       <c r="T44" s="8">
         <v>0.03</v>
@@ -3418,7 +3418,7 @@
         <v>-9.2347845519760007E-3</v>
       </c>
       <c r="S45" s="8">
-        <v>-212.34351461449799</v>
+        <v>-3.9284729884809999E-3</v>
       </c>
       <c r="T45" s="8">
         <v>0.03</v>
@@ -3483,7 +3483,7 @@
         <v>-1.4624549191928999E-2</v>
       </c>
       <c r="S46" s="8">
-        <v>-116.727437593283</v>
+        <v>-8.5042551028300002E-4</v>
       </c>
       <c r="T46" s="8">
         <v>3.1166666666666665E-2</v>
@@ -3548,7 +3548,7 @@
         <v>-7.2262018876399997E-4</v>
       </c>
       <c r="S47" s="8">
-        <v>-185.97885108438601</v>
+        <v>-2.428123176438E-3</v>
       </c>
       <c r="T47" s="8">
         <v>3.7802197802197804E-2</v>
@@ -3613,7 +3613,7 @@
         <v>-3.2080726383550001E-3</v>
       </c>
       <c r="S48" s="8">
-        <v>921.38284693594301</v>
+        <v>2.7209376164514E-2</v>
       </c>
       <c r="T48" s="8">
         <v>4.4157608695652176E-2</v>
@@ -3678,7 +3678,7 @@
         <v>1.2003798375100001E-3</v>
       </c>
       <c r="S49" s="8">
-        <v>666.72571321779799</v>
+        <v>2.0369812044546E-2</v>
       </c>
       <c r="T49" s="8">
         <v>4.5923913043478259E-2</v>
@@ -3743,7 +3743,7 @@
         <v>2.421546515462E-3</v>
       </c>
       <c r="S50" s="8">
-        <v>-1095.42139260203</v>
+        <v>-2.5693722279524999E-2</v>
       </c>
       <c r="T50" s="8">
         <v>5.0109890109890108E-2</v>
@@ -3808,7 +3808,7 @@
         <v>1.0474364185300001E-3</v>
       </c>
       <c r="S51" s="8">
-        <v>-213.248944681734</v>
+        <v>-2.3991846150830001E-3</v>
       </c>
       <c r="T51" s="8">
         <v>5.2499999999999998E-2</v>
@@ -3873,7 +3873,7 @@
         <v>2.1816486960110001E-3</v>
       </c>
       <c r="S52" s="8">
-        <v>-880.10316634015896</v>
+        <v>-1.9315792445468001E-2</v>
       </c>
       <c r="T52" s="8">
         <v>4.9836956521739133E-2</v>
@@ -3938,7 +3938,7 @@
         <v>1.254201326406E-3</v>
       </c>
       <c r="S53" s="8">
-        <v>-1871.4753732357001</v>
+        <v>-4.4404941380257003E-2</v>
       </c>
       <c r="T53" s="8">
         <v>4.6304347826086951E-2</v>
@@ -4003,7 +4003,7 @@
         <v>6.1214757320089998E-3</v>
       </c>
       <c r="S54" s="8">
-        <v>109.0679435056</v>
+        <v>5.241660528993E-3</v>
       </c>
       <c r="T54" s="8">
         <v>3.9472222222222221E-2</v>
@@ -4068,7 +4068,7 @@
         <v>1.1753634705998999E-2</v>
       </c>
       <c r="S55" s="8">
-        <v>-738.01948259749702</v>
+        <v>-1.5492956605545E-2</v>
       </c>
       <c r="T55" s="8">
         <v>3.2500000000000001E-2</v>
@@ -4133,7 +4133,7 @@
         <v>8.0478879273440003E-3</v>
       </c>
       <c r="S56" s="8">
-        <v>-1757.0000361653199</v>
+        <v>-4.0348868186530003E-2</v>
       </c>
       <c r="T56" s="8">
         <v>3.2500000000000001E-2</v>
@@ -4198,7 +4198,7 @@
         <v>1.1729591708117999E-2</v>
       </c>
       <c r="S57" s="8">
-        <v>1617.6274015015899</v>
+        <v>3.8619507609687999E-2</v>
       </c>
       <c r="T57" s="8">
         <v>3.2500000000000001E-2</v>
@@ -4263,7 +4263,7 @@
         <v>1.1991017150622001E-2</v>
       </c>
       <c r="S58" s="8">
-        <v>1229.0372038937301</v>
+        <v>2.9138860980253999E-2</v>
       </c>
       <c r="T58" s="8">
         <v>3.2500000000000001E-2</v>
@@ -4328,7 +4328,7 @@
         <v>1.0277100257367E-2</v>
       </c>
       <c r="S59" s="8">
-        <v>1308.2561919163099</v>
+        <v>3.0199469122347999E-2</v>
       </c>
       <c r="T59" s="8">
         <v>3.5219780219780221E-2</v>
@@ -4393,7 +4393,7 @@
         <v>8.5589450427510008E-3</v>
       </c>
       <c r="S60" s="8">
-        <v>1921.8697163464301</v>
+        <v>4.2879475041728003E-2</v>
       </c>
       <c r="T60" s="8">
         <v>4.2472826086956524E-2</v>
@@ -4458,7 +4458,7 @@
         <v>1.8294781193957999E-2</v>
       </c>
       <c r="S61" s="8">
-        <v>1945.7171611568001</v>
+        <v>4.2684090913429E-2</v>
       </c>
       <c r="T61" s="8">
         <v>4.4999999999999998E-2</v>
@@ -4523,7 +4523,7 @@
         <v>1.5732875955937E-2</v>
       </c>
       <c r="S62" s="8">
-        <v>1917.5690020776999</v>
+        <v>4.1478071896491997E-2</v>
       </c>
       <c r="T62" s="8">
         <v>4.4999999999999998E-2</v>
@@ -4588,7 +4588,7 @@
         <v>1.5650906221762E-2</v>
       </c>
       <c r="S63" s="8">
-        <v>2227.5514225429501</v>
+        <v>4.7515067371199003E-2</v>
       </c>
       <c r="T63" s="8">
         <v>4.4999999999999998E-2</v>
@@ -4653,7 +4653,7 @@
         <v>2.4366066458926E-2</v>
       </c>
       <c r="S64" s="8">
-        <v>2226.3075304756799</v>
+        <v>4.7091634950741E-2</v>
       </c>
       <c r="T64" s="8">
         <v>4.5081521739130437E-2</v>
@@ -4718,7 +4718,7 @@
         <v>-8.0962288069930007E-3</v>
       </c>
       <c r="S65" s="8">
-        <v>-433.57591641119501</v>
+        <v>-1.0022689299904E-2</v>
       </c>
       <c r="T65" s="8">
         <v>5.1874999999999998E-2</v>
@@ -4783,7 +4783,7 @@
         <v>3.17406667712E-3</v>
       </c>
       <c r="S66" s="8">
-        <v>-896.62466027386097</v>
+        <v>-2.0141470023225E-2</v>
       </c>
       <c r="T66" s="8">
         <v>6.0494505494505496E-2</v>
@@ -4848,7 +4848,7 @@
         <v>-5.5428534642300005E-4</v>
       </c>
       <c r="S67" s="8">
-        <v>-494.70648615375802</v>
+        <v>-1.1112156263188001E-2</v>
       </c>
       <c r="T67" s="8">
         <v>6.9368131868131871E-2</v>
@@ -4913,7 +4913,7 @@
         <v>-4.1637925252630001E-3</v>
       </c>
       <c r="S68" s="8">
-        <v>-1547.01181472339</v>
+        <v>-3.4108539090558998E-2</v>
       </c>
       <c r="T68" s="8">
         <v>7.6657608695652177E-2</v>
@@ -4978,7 +4978,7 @@
         <v>-4.5263339411200001E-3</v>
       </c>
       <c r="S69" s="8">
-        <v>730.35341772525101</v>
+        <v>1.5858442340088E-2</v>
       </c>
       <c r="T69" s="8">
         <v>7.714673913043478E-2</v>
@@ -5043,7 +5043,7 @@
         <v>-8.0484467168699999E-3</v>
       </c>
       <c r="S70" s="8">
-        <v>-431.69687550432701</v>
+        <v>-8.729186665136E-3</v>
       </c>
       <c r="T70" s="8">
         <v>7.3944444444444452E-2</v>
@@ -5108,7 +5108,7 @@
         <v>-5.2897019577930002E-3</v>
       </c>
       <c r="S71" s="8">
-        <v>-253.24825949385499</v>
+        <v>-4.3610409269289998E-3</v>
       </c>
       <c r="T71" s="8">
         <v>6.5824175824175823E-2</v>
@@ -5173,7 +5173,7 @@
         <v>-5.6164939323740002E-3</v>
       </c>
       <c r="S72" s="8">
-        <v>768.30720910343302</v>
+        <v>1.8149920368892E-2</v>
       </c>
       <c r="T72" s="8">
         <v>5.5081521739130439E-2</v>
@@ -5238,7 +5238,7 @@
         <v>-8.1306844088860006E-3</v>
       </c>
       <c r="S73" s="8">
-        <v>833.93467852767196</v>
+        <v>2.0197268135343002E-2</v>
       </c>
       <c r="T73" s="8">
         <v>4.9836956521739133E-2</v>
@@ -5303,7 +5303,7 @@
         <v>8.230760965E-4</v>
       </c>
       <c r="S74" s="8">
-        <v>-984.87515869316803</v>
+        <v>-1.8640552621775001E-2</v>
       </c>
       <c r="T74" s="8">
         <v>4.5805555555555558E-2</v>
@@ -5368,7 +5368,7 @@
         <v>3.6771357582489998E-3</v>
       </c>
       <c r="S75" s="8">
-        <v>1449.7404316025199</v>
+        <v>3.4744339027989998E-2</v>
       </c>
       <c r="T75" s="8">
         <v>4.3296703296703293E-2</v>
@@ -5433,7 +5433,7 @@
         <v>2.39468829623E-3</v>
       </c>
       <c r="S76" s="8">
-        <v>1933.86434608585</v>
+        <v>4.5772038186897998E-2</v>
       </c>
       <c r="T76" s="8">
         <v>4.2500000000000003E-2</v>
@@ -5498,7 +5498,7 @@
         <v>2.6802590847819999E-3</v>
       </c>
       <c r="S77" s="8">
-        <v>2276.7682999337198</v>
+        <v>5.3842195911382999E-2</v>
       </c>
       <c r="T77" s="8">
         <v>4.2500000000000003E-2</v>
@@ -5563,7 +5563,7 @@
         <v>4.2879737787479997E-3</v>
       </c>
       <c r="S78" s="8">
-        <v>3123.92486663821</v>
+        <v>7.2377533105886002E-2</v>
       </c>
       <c r="T78" s="8">
         <v>4.2500000000000003E-2</v>
@@ -5628,7 +5628,7 @@
         <v>9.3693503971599996E-3</v>
       </c>
       <c r="S79" s="8">
-        <v>4214.9013779277502</v>
+        <v>9.5700761747087998E-2</v>
       </c>
       <c r="T79" s="8">
         <v>4.2500000000000003E-2</v>
@@ -5693,7 +5693,7 @@
         <v>1.1780333030908001E-2</v>
       </c>
       <c r="S80" s="8">
-        <v>3760.99774710882</v>
+        <v>8.7405272145896995E-2</v>
       </c>
       <c r="T80" s="8">
         <v>4.2500000000000003E-2</v>
@@ -5758,7 +5758,7 @@
         <v>1.822658694498E-2</v>
       </c>
       <c r="S81" s="8">
-        <v>1221.9066194679399</v>
+        <v>3.4318555953296997E-2</v>
       </c>
       <c r="T81" s="8">
         <v>4.2500000000000003E-2</v>
@@ -5823,7 +5823,7 @@
         <v>5.5417460049229997E-3</v>
       </c>
       <c r="S82" s="8">
-        <v>-1995.0237969879599</v>
+        <v>-3.8446609162106002E-2</v>
       </c>
       <c r="T82" s="8">
         <v>4.2390109890109891E-2</v>
@@ -5888,7 +5888,7 @@
         <v>-0.18412146420574299</v>
       </c>
       <c r="S83" s="8">
-        <v>-15184.232344391799</v>
+        <v>-0.41394236483556301</v>
       </c>
       <c r="T83" s="8">
         <v>3.2664835164835163E-2</v>
@@ -5953,7 +5953,7 @@
         <v>-0.10614015924358</v>
       </c>
       <c r="S84" s="8">
-        <v>-7426.6389480768903</v>
+        <v>-0.17737911391522801</v>
       </c>
       <c r="T84" s="8">
         <v>2.2499999999999999E-2</v>
@@ -6018,7 +6018,7 @@
         <v>-1.3417251269726999E-2</v>
       </c>
       <c r="S85" s="8">
-        <v>-4849.7974687144597</v>
+        <v>-0.10976477784996801</v>
       </c>
       <c r="T85" s="8">
         <v>1.7500000000000002E-2</v>
@@ -6083,7 +6083,7 @@
         <v>-2.3972114782269999E-3</v>
       </c>
       <c r="S86" s="8">
-        <v>-53.570709826482897</v>
+        <v>6.102873641478E-3</v>
       </c>
       <c r="T86" s="8">
         <v>1.7500000000000002E-2</v>
@@ -6148,7 +6148,7 @@
         <v>-3.3078034877475002E-2</v>
       </c>
       <c r="S87" s="8">
-        <v>-2479.4785166004999</v>
+        <v>-5.1536899983500001E-2</v>
       </c>
       <c r="T87" s="8">
         <v>1.7500000000000002E-2</v>
@@ -6213,7 +6213,7 @@
         <v>1.57281471127E-2</v>
       </c>
       <c r="S88" s="8">
-        <v>-1410.1683829092799</v>
+        <v>-2.6291322487098999E-2</v>
       </c>
       <c r="T88" s="8">
         <v>1.7500000000000002E-2</v>
@@ -6278,7 +6278,7 @@
         <v>5.8626232837662003E-2</v>
       </c>
       <c r="S89" s="8">
-        <v>918.00050728187398</v>
+        <v>2.7112168428212999E-2</v>
       </c>
       <c r="T89" s="8">
         <v>2.391304347826087E-2</v>
@@ -6343,7 +6343,7 @@
         <v>5.7428737618368003E-2</v>
       </c>
       <c r="S90" s="8">
-        <v>4314.2100172684704</v>
+        <v>0.10046688739456799</v>
       </c>
       <c r="T90" s="8">
         <v>3.6666666666666667E-2</v>
@@ -6408,7 +6408,7 @@
         <v>5.6791368736457001E-2</v>
       </c>
       <c r="S91" s="8">
-        <v>3542.7482485648802</v>
+        <v>8.3800209319867994E-2</v>
       </c>
       <c r="T91" s="8">
         <v>5.6593406593406594E-2</v>
@@ -6473,7 +6473,7 @@
         <v>4.8100508080120001E-2</v>
       </c>
       <c r="S92" s="8">
-        <v>4807.5350948101704</v>
+        <v>0.11003739383911799</v>
       </c>
       <c r="T92" s="8">
         <v>8.5054347826086951E-2</v>
@@ -6538,7 +6538,7 @@
         <v>3.3386017802921997E-2</v>
       </c>
       <c r="S93" s="8">
-        <v>4881.0988587639804</v>
+        <v>0.111220789903795</v>
       </c>
       <c r="T93" s="8">
         <v>0.10815217391304348</v>
@@ -6603,7 +6603,7 @@
         <v>2.8572212895709999E-2</v>
       </c>
       <c r="S94" s="8">
-        <v>1441.9436555254199</v>
+        <v>3.6665898525457999E-2</v>
       </c>
       <c r="T94" s="8">
         <v>0.12511111111111112</v>
@@ -6668,7 +6668,7 @@
         <v>1.4061135490214E-2</v>
       </c>
       <c r="S95" s="8">
-        <v>-1338.7661074274999</v>
+        <v>-2.823432886607E-2</v>
       </c>
       <c r="T95" s="8">
         <v>0.13164835164835165</v>
@@ -6733,7 +6733,7 @@
         <v>6.4187579733130003E-3</v>
       </c>
       <c r="S96" s="8">
-        <v>-2146.10973660833</v>
+        <v>-4.8378578761213001E-2</v>
       </c>
       <c r="T96" s="8">
         <v>0.13250000000000001</v>
@@ -6798,7 +6798,7 @@
         <v>-7.204704654214E-3</v>
       </c>
       <c r="S97" s="8">
-        <v>-3528.3369968440702</v>
+        <v>-8.3480428412290003E-2</v>
       </c>
       <c r="T97" s="8">
         <v>0.13217391304347825</v>
@@ -6863,7 +6863,7 @@
         <v>-1.3483969772471001E-2</v>
       </c>
       <c r="S98" s="8">
-        <v>-791.68682668119402</v>
+        <v>-1.6922578286943001E-2</v>
       </c>
       <c r="T98" s="8">
         <v>0.12802197802197804</v>
@@ -6928,7 +6928,7 @@
         <v>-1.3201529303484999E-2</v>
       </c>
       <c r="S99" s="8">
-        <v>-171.689879501711</v>
+        <v>-2.8371075995789999E-3</v>
       </c>
       <c r="T99" s="8">
         <v>0.1192032967032967</v>
@@ -6993,7 +6993,7 @@
         <v>-2.2376234557686999E-2</v>
       </c>
       <c r="S100" s="8">
-        <v>247.734043274962</v>
+        <v>6.4298520553870003E-3</v>
       </c>
       <c r="T100" s="8">
         <v>0.10923913043478262</v>
@@ -7058,7 +7058,7 @@
         <v>-1.4852320654592001E-2</v>
       </c>
       <c r="S101" s="8">
-        <v>1721.4650325216501</v>
+        <v>3.9697854682614997E-2</v>
       </c>
       <c r="T101" s="8">
         <v>9.8940217391304361E-2</v>
@@ -7123,7 +7123,7 @@
         <v>-1.4187647759005001E-2</v>
       </c>
       <c r="S102" s="8">
-        <v>-533.67877244997999</v>
+        <v>-1.3064867371782999E-2</v>
       </c>
       <c r="T102" s="8">
         <v>9.5000000000000001E-2</v>

</xml_diff>

<commit_message>
Adds observable for nominal interest rate
</commit_message>
<xml_diff>
--- a/08_Pronóstico/Datos/DataCOL.xlsx
+++ b/08_Pronóstico/Datos/DataCOL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarincong/Documents/Git Repos/CAEP/08_Pronóstico/Datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{991E9AE8-93F8-9943-87C5-508AEDEF052B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871CF68F-5E43-E84A-8459-5816B236E151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1000" windowWidth="28080" windowHeight="21100" xr2:uid="{3B812F19-A572-41B0-90ED-022F2B941229}"/>
   </bookViews>
@@ -47,6 +47,9 @@
     <t>I_obs</t>
   </si>
   <si>
+    <t>i_nom_obs</t>
+  </si>
+  <si>
     <t>Y</t>
   </si>
   <si>
@@ -66,9 +69,6 @@
   </si>
   <si>
     <t>P_d</t>
-  </si>
-  <si>
-    <t>i_nom</t>
   </si>
   <si>
     <t>Dates</t>
@@ -476,9 +476,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC43C700-5E37-433E-91EB-5805D755A630}">
   <dimension ref="A1:AC111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="150" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S13" sqref="S13"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="150" zoomScaleNormal="160" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O81" sqref="O81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -506,7 +506,7 @@
         <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
         <v>16</v>
@@ -515,31 +515,31 @@
         <v>13</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F1" t="s">
         <v>14</v>
       </c>
       <c r="G1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H1" t="s">
         <v>15</v>
       </c>
       <c r="I1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J1" t="s">
         <v>12</v>
       </c>
       <c r="K1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N1" t="s">
         <v>17</v>
@@ -560,7 +560,7 @@
         <v>2</v>
       </c>
       <c r="T1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="X1" s="3"/>
       <c r="Y1" s="3"/>

</xml_diff>

<commit_message>
Estimation of Exogenous variables Standard Deviations
</commit_message>
<xml_diff>
--- a/08_Pronóstico/Datos/DataCOL.xlsx
+++ b/08_Pronóstico/Datos/DataCOL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarincong/Documents/Git Repos/CAEP/08_Pronóstico/Datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871CF68F-5E43-E84A-8459-5816B236E151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B6ADA5-82F3-324D-873A-30290B0389DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1000" windowWidth="28080" windowHeight="21100" xr2:uid="{3B812F19-A572-41B0-90ED-022F2B941229}"/>
   </bookViews>
@@ -74,9 +74,6 @@
     <t>Dates</t>
   </si>
   <si>
-    <t>pi</t>
-  </si>
-  <si>
     <t>y_star_obs</t>
   </si>
   <si>
@@ -96,6 +93,9 @@
   </si>
   <si>
     <t>I_obs Lev</t>
+  </si>
+  <si>
+    <t>pi_obs</t>
   </si>
 </sst>
 </file>
@@ -476,9 +476,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC43C700-5E37-433E-91EB-5805D755A630}">
   <dimension ref="A1:AC111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="150" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O81" sqref="O81"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="150" zoomScaleNormal="160" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J3" sqref="J3:J103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -509,28 +509,28 @@
         <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
         <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G1" t="s">
         <v>8</v>
       </c>
       <c r="H1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I1" t="s">
         <v>10</v>
       </c>
       <c r="J1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="K1" t="s">
         <v>4</v>
@@ -542,13 +542,13 @@
         <v>6</v>
       </c>
       <c r="N1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" t="s">
         <v>17</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>18</v>
-      </c>
-      <c r="P1" t="s">
-        <v>19</v>
       </c>
       <c r="Q1" t="s">
         <v>0</v>

</xml_diff>